<commit_message>
Atualização na construção do aplicativo
</commit_message>
<xml_diff>
--- a/contatosMay.xlsx
+++ b/contatosMay.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:D3"/>
+  <dimension ref="A1:D4"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -466,12 +466,12 @@
       </c>
       <c r="C2" t="inlineStr">
         <is>
-          <t>Boa tarde</t>
+          <t>teste</t>
         </is>
       </c>
       <c r="D2" t="inlineStr">
         <is>
-          <t>Chegou a sua vez, aproveite!</t>
+          <t>zap</t>
         </is>
       </c>
     </row>
@@ -486,12 +486,32 @@
       </c>
       <c r="C3" t="inlineStr">
         <is>
-          <t>Boa tarde</t>
+          <t>teste</t>
         </is>
       </c>
       <c r="D3" t="inlineStr">
         <is>
-          <t>Chegou a sua vez, aproveite!</t>
+          <t>zap</t>
+        </is>
+      </c>
+    </row>
+    <row r="4">
+      <c r="A4" t="inlineStr">
+        <is>
+          <t>Cristian</t>
+        </is>
+      </c>
+      <c r="B4" t="n">
+        <v>5543996777718</v>
+      </c>
+      <c r="C4" t="inlineStr">
+        <is>
+          <t>teste</t>
+        </is>
+      </c>
+      <c r="D4" t="inlineStr">
+        <is>
+          <t>zap</t>
         </is>
       </c>
     </row>

</xml_diff>

<commit_message>
Apagando arquivos de teste
</commit_message>
<xml_diff>
--- a/contatosMay.xlsx
+++ b/contatosMay.xlsx
@@ -464,11 +464,7 @@
       <c r="B2" t="n">
         <v>5541984988524</v>
       </c>
-      <c r="C2" t="inlineStr">
-        <is>
-          <t>teste</t>
-        </is>
-      </c>
+      <c r="C2" t="inlineStr"/>
       <c r="D2" t="inlineStr">
         <is>
           <t>zap</t>

</xml_diff>